<commit_message>
Fix excel. Mobile login
</commit_message>
<xml_diff>
--- a/packages/server/public/default/Preguntas_FORMATO.xlsx
+++ b/packages/server/public/default/Preguntas_FORMATO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PREGUNTAS" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">PREGUNTA</t>
   </si>
   <si>
     <t xml:space="preserve">COMENTARIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIVEL</t>
   </si>
   <si>
     <t xml:space="preserve">¿Qué principios tienen relacion de género a especie?</t>
@@ -182,9 +185,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -288,38 +295,47 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="167.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="126.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -340,11 +356,11 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="72.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.43"/>
@@ -352,91 +368,91 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="B2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6"/>
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>